<commit_message>
Correção no estudo de viabilidade proposto pelo professor.
Documentos para armazenamento
</commit_message>
<xml_diff>
--- a/TCC/Cronograma.xlsx
+++ b/TCC/Cronograma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Inicio</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Alisson</t>
+  </si>
+  <si>
+    <t>Organograma</t>
   </si>
 </sst>
 </file>
@@ -185,34 +188,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,58 +514,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>44775</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -577,10 +581,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>44775</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" t="s">
         <v>10</v>
       </c>
@@ -591,15 +595,15 @@
         <v>1</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ref="F6:F8" si="0">IF(E6&lt;=30%,"Primicias",IF(E6&lt;5=50%,"Em Desenvolvimento",IF(E6&lt;=99%,"No finalmente","Concluido")))</f>
+        <f t="shared" ref="F6:F9" si="0">IF(E6&lt;=30%,"Primicias",IF(E6&lt;5=50%,"Em Desenvolvimento",IF(E6&lt;=99%,"No finalmente","Concluido")))</f>
         <v>Concluido</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>44775</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" t="s">
         <v>13</v>
       </c>
@@ -635,8 +639,28 @@
         <v>Concluido</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>44796</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>Concluido</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
Cronograma tcc e estudo de viabilidade
</commit_message>
<xml_diff>
--- a/TCC/Cronograma.xlsx
+++ b/TCC/Cronograma.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorio\Etec\TCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Etec\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1706A3C-0F3C-43EE-9291-E0FA1B9E47F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Inicio</t>
   </si>
@@ -96,13 +95,16 @@
   </si>
   <si>
     <t>Criação e elaboração do Histórico, Missão, Visão, Valores referente a empresa cliente</t>
+  </si>
+  <si>
+    <t>Banco de Dados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,16 +119,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -207,41 +223,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -260,6 +309,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1295400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5391150" y="0"/>
+          <a:ext cx="1295400" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -524,222 +622,242 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" customWidth="1"/>
+    <col min="1" max="2" width="12.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="11">
         <v>44775</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="12">
         <v>1</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F5" s="7" t="str">
         <f>IF(E5&lt;=30%,"Primicias",IF(E5&lt;5=50%,"Em Desenvolvimento",IF(E5&lt;=99%,"No finalmente","Concluido")))</f>
         <v>Concluido</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="11">
         <v>44775</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="12">
         <v>1</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" ref="F6:F12" si="0">IF(E6&lt;=30%,"Primicias",IF(E6&lt;5=50%,"Em Desenvolvimento",IF(E6&lt;=99%,"No finalmente","Concluido")))</f>
+      <c r="F6" s="7" t="str">
+        <f t="shared" ref="F6:F13" si="0">IF(E6&lt;=30%,"Primicias",IF(E6&lt;5=50%,"Em Desenvolvimento",IF(E6&lt;=99%,"No finalmente","Concluido")))</f>
         <v>Concluido</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="11">
         <v>44775</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="12">
         <v>1</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="13">
         <v>44786</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="13">
         <v>44789</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="12">
         <v>1</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="11">
         <v>44796</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="12">
         <v>1</v>
       </c>
-      <c r="F9" s="4" t="str">
+      <c r="F9" s="14" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="11">
         <v>44817</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="12">
         <v>1</v>
       </c>
-      <c r="F10" s="4" t="str">
+      <c r="F10" s="14" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="11">
         <v>44820</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="12">
         <v>1</v>
       </c>
-      <c r="F11" s="4" t="str">
+      <c r="F11" s="14" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="11">
         <v>44820</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="12">
         <v>1</v>
       </c>
-      <c r="F12" s="4" t="str">
+      <c r="F12" s="14" t="str">
         <f t="shared" si="0"/>
         <v>Concluido</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>44822</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>No finalmente</v>
       </c>
     </row>
   </sheetData>
@@ -749,13 +867,15 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>